<commit_message>
Added stp files for updated MM components
</commit_message>
<xml_diff>
--- a/hw/PCB/KICAD/R21_Core/R21_Core_BOM.xlsx
+++ b/hw/PCB/KICAD/R21_Core/R21_Core_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="2940" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="2720" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,9 +451,6 @@
     <t>CRYSTAL 16.0000MHZ 10PF SMD</t>
   </si>
   <si>
-    <t>ABM3B-16.000MHZ-10-1-U-T</t>
-  </si>
-  <si>
     <t>C28,C41</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>J1</t>
+  </si>
+  <si>
+    <t>ABM8-16.000MHZ-10-1-U-T</t>
   </si>
 </sst>
 </file>
@@ -539,8 +539,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -559,13 +563,17 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -897,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -980,7 +988,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -994,7 +1002,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1134,7 +1142,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1218,7 +1226,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1470,16 +1478,16 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" t="s">
         <v>152</v>
-      </c>
-      <c r="D41" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1498,7 +1506,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -1610,16 +1618,16 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1633,7 +1641,7 @@
         <v>142</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:4">

</xml_diff>

<commit_message>
long time since commit
</commit_message>
<xml_diff>
--- a/hw/PCB/KICAD/R21_Core/R21_Core_BOM.xlsx
+++ b/hw/PCB/KICAD/R21_Core/R21_Core_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="2720" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2720" windowWidth="64000" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -539,8 +539,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -563,17 +567,21 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -905,13 +913,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="74.5" customWidth="1"/>
     <col min="3" max="3" width="54.5" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>